<commit_message>
Fixed long legend label
</commit_message>
<xml_diff>
--- a/professions_hommes.xlsx
+++ b/professions_hommes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AubertSigouin-Lebel\Documents\dsviz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{67974988-AE38-4346-AAD9-8E2AC41129F4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08D0D46-B5B6-4BCE-8126-2821B60C408E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18840" windowHeight="5810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t xml:space="preserve">  9222 Surveillants dans la fabrication de matériel électronique</t>
   </si>
   <si>
-    <t xml:space="preserve">  9523 Assembleurs, monteurs, contrôleurs et vérificateurs de matériel électronique</t>
-  </si>
-  <si>
     <t>Géographie:  Québec</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">  7202 Entrepreneurs et contremaîtres en électricité et en télécommunications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  9523 Assembleurs, monteurs, contrôleurs et vérificateurs de matériel électronique             </t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -477,13 +477,13 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -544,7 +544,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1277,7 +1277,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>2.5</v>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>10.7</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>3.8</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>5.5</v>

</xml_diff>

<commit_message>
Changed CNP9 hommes femmes
</commit_message>
<xml_diff>
--- a/professions_hommes.xlsx
+++ b/professions_hommes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AubertSigouin-Lebel\Documents\dsviz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08D0D46-B5B6-4BCE-8126-2821B60C408E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7945DA-CA02-4E77-B5A6-5A69109D6195}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18840" windowHeight="5810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">  7202 Entrepreneurs et contremaîtres en électricité et en télécommunications</t>
   </si>
   <si>
-    <t xml:space="preserve">  9523 Assembleurs, monteurs, contrôleurs et vérificateurs de matériel électronique             </t>
+    <t xml:space="preserve">  9523 Assembleurs, monteurs, contrôleurs et vérificateurs de matériel électronique    </t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>

</xml_diff>